<commit_message>
Latest Member List Update
</commit_message>
<xml_diff>
--- a/5.23-5.29.xlsx
+++ b/5.23-5.29.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="164">
   <si>
     <t>ID</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>Test</t>
-  </si>
-  <si>
-    <t>TEST</t>
   </si>
   <si>
     <t>KILL</t>
@@ -898,13 +895,15 @@
   <dimension ref="A1:S113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -986,10 +985,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
+        <v>48</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -997,7 +999,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1005,7 +1013,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1013,7 +1027,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="E6" s="8">
+        <v>4</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1021,7 +1041,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="E7" s="8">
+        <v>5</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1029,7 +1055,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="E8" s="8">
+        <v>6</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1037,7 +1069,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="E9" s="8">
+        <v>7</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1045,7 +1083,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="E10" s="8">
+        <v>8</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1053,7 +1097,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="E11" s="8">
+        <v>9</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1061,7 +1111,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="E12" s="8">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1069,7 +1125,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="E13" s="8">
+        <v>11</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1077,7 +1139,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="E14" s="8">
+        <v>12</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1085,7 +1153,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="E15" s="8">
+        <v>13</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1093,519 +1167,861 @@
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="E16" s="8">
+        <v>14</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="E17" s="8">
+        <v>15</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="E18" s="8">
+        <v>16</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="E19" s="8">
+        <v>17</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="E20" s="8">
+        <v>18</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="E21" s="8">
+        <v>19</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E22" s="8">
+        <v>20</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E23" s="8">
+        <v>21</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="E24" s="8">
+        <v>22</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="E25" s="8">
+        <v>23</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="E26" s="8">
+        <v>24</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="E27" s="8">
+        <v>25</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="E28" s="8">
+        <v>26</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="E29" s="8">
+        <v>27</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="E30" s="8">
+        <v>28</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="E31" s="8">
+        <v>29</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>30</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E32" s="8">
+        <v>30</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>31</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="E33" s="8">
+        <v>31</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>32</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="E34" s="8">
+        <v>32</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="E35" s="8">
+        <v>33</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>34</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="E36" s="8">
+        <v>34</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="E37" s="8">
+        <v>35</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>36</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="E38" s="8">
+        <v>36</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>37</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="E39" s="8">
+        <v>37</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="E40" s="8">
+        <v>38</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>39</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="E41" s="8">
+        <v>39</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>40</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="E42" s="8">
+        <v>40</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>41</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E43" s="8">
+        <v>41</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="E44" s="8">
+        <v>42</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>43</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="E45" s="8">
+        <v>43</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>44</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="E46" s="8">
+        <v>44</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>45</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="E47" s="8">
+        <v>45</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>46</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E48" s="8">
+        <v>46</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>47</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="E49" s="8">
+        <v>47</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>48</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="E50" s="8">
+        <v>48</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>49</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="E51" s="8">
+        <v>49</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>50</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="E52" s="8">
+        <v>50</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>51</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="E53" s="8">
+        <v>51</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>52</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="E54" s="8">
+        <v>52</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>53</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="E55" s="8">
+        <v>53</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>54</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="E56" s="8">
+        <v>54</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>55</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="E57" s="8">
+        <v>55</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>56</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="E58" s="8">
+        <v>56</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>57</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="E59" s="8">
+        <v>57</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>58</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E60" s="8">
+        <v>58</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>59</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="E61" s="8">
+        <v>59</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>60</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="E62" s="8">
+        <v>60</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>61</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E63" s="8">
+        <v>61</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>62</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="E64" s="8">
+        <v>62</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>63</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="E65" s="8">
+        <v>63</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>64</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="E66" s="8">
+        <v>64</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>65</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="E67" s="8">
+        <v>65</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>66</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="E68" s="8">
+        <v>66</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>67</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="E69" s="8">
+        <v>67</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>68</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="E70" s="8">
+        <v>68</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>69</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="E71" s="8">
+        <v>69</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>70</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="E72" s="8">
+        <v>70</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>71</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>72</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>73</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>74</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>75</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>76</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>77</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <v>78</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1613,7 +2029,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1621,7 +2037,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1629,7 +2045,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1637,7 +2053,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1645,7 +2061,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1653,7 +2069,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1661,7 +2077,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1669,7 +2085,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1677,7 +2093,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1685,7 +2101,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1693,7 +2109,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1701,7 +2117,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1709,7 +2125,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1717,7 +2133,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1725,7 +2141,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1733,7 +2149,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1741,7 +2157,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1749,7 +2165,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1757,7 +2173,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1765,7 +2181,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1773,7 +2189,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -1781,7 +2197,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -1789,7 +2205,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -1797,7 +2213,7 @@
         <v>102</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -1805,7 +2221,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -1813,7 +2229,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -1821,7 +2237,7 @@
         <v>105</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -1829,7 +2245,7 @@
         <v>106</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -1837,7 +2253,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -1845,7 +2261,7 @@
         <v>108</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -1853,7 +2269,7 @@
         <v>109</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -1861,7 +2277,7 @@
         <v>110</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -1869,7 +2285,7 @@
         <v>111</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1966,7 +2382,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1988,45 +2404,45 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="9">
         <v>2</v>
@@ -2036,7 +2452,7 @@
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="9">
         <v>1</v>
@@ -2046,7 +2462,7 @@
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4" s="9">
         <v>2</v>
@@ -2056,7 +2472,7 @@
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N4" s="9">
         <v>4</v>
@@ -2067,7 +2483,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="9">
         <v>7</v>
@@ -2077,7 +2493,7 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="9">
         <v>6</v>
@@ -2087,7 +2503,7 @@
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J5" s="10">
         <v>0</v>
@@ -2097,7 +2513,7 @@
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N5" s="10">
         <v>7</v>
@@ -2108,7 +2524,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="9">
         <v>2</v>
@@ -2118,7 +2534,7 @@
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="9">
         <v>14</v>
@@ -2128,7 +2544,7 @@
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6" s="10">
         <v>1</v>
@@ -2138,7 +2554,7 @@
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N6" s="10">
         <v>7</v>
@@ -2149,7 +2565,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="9">
         <v>19</v>
@@ -2159,7 +2575,7 @@
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="9">
         <v>16</v>
@@ -2169,7 +2585,7 @@
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J7" s="9">
         <v>0</v>
@@ -2179,7 +2595,7 @@
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N7" s="10">
         <v>0</v>
@@ -2190,7 +2606,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="9">
         <v>0</v>
@@ -2200,7 +2616,7 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="9">
         <v>0</v>
@@ -2210,7 +2626,7 @@
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J8" s="9">
         <v>15</v>
@@ -2220,7 +2636,7 @@
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N8" s="10">
         <v>6</v>
@@ -2231,7 +2647,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="9">
         <v>4</v>
@@ -2241,7 +2657,7 @@
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" s="9">
         <v>13</v>
@@ -2251,7 +2667,7 @@
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J9" s="9">
         <v>19</v>
@@ -2261,7 +2677,7 @@
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N9" s="9">
         <v>7</v>
@@ -2272,7 +2688,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="9">
         <v>15</v>
@@ -2282,7 +2698,7 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" s="10">
         <v>4</v>
@@ -2292,7 +2708,7 @@
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J10" s="9">
         <v>1</v>
@@ -2302,7 +2718,7 @@
       </c>
       <c r="L10" s="8"/>
       <c r="M10" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N10" s="9">
         <v>12</v>
@@ -2313,7 +2729,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="9">
         <v>2</v>
@@ -2323,7 +2739,7 @@
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="9">
         <v>14</v>
@@ -2333,7 +2749,7 @@
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J11" s="9">
         <v>6</v>
@@ -2343,7 +2759,7 @@
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N11" s="9">
         <v>1</v>
@@ -2354,7 +2770,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="9">
         <v>0</v>
@@ -2364,7 +2780,7 @@
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="9">
         <v>4</v>
@@ -2374,7 +2790,7 @@
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J12" s="9">
         <v>5</v>
@@ -2384,7 +2800,7 @@
       </c>
       <c r="L12" s="8"/>
       <c r="M12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N12" s="10">
         <v>7</v>
@@ -2395,7 +2811,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="9">
         <v>5</v>
@@ -2405,7 +2821,7 @@
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F13" s="9">
         <v>1</v>
@@ -2415,7 +2831,7 @@
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J13" s="9">
         <v>2</v>
@@ -2425,7 +2841,7 @@
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N13" s="10">
         <v>2</v>
@@ -2436,7 +2852,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="9">
         <v>4</v>
@@ -2446,7 +2862,7 @@
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F14" s="9">
         <v>1</v>
@@ -2456,7 +2872,7 @@
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J14" s="9">
         <v>1</v>
@@ -2466,7 +2882,7 @@
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N14" s="9">
         <v>11</v>
@@ -2477,7 +2893,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="9">
         <v>4</v>
@@ -2487,7 +2903,7 @@
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" s="9">
         <v>20</v>
@@ -2497,7 +2913,7 @@
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J15" s="9">
         <v>15</v>
@@ -2507,7 +2923,7 @@
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N15" s="10">
         <v>5</v>
@@ -2518,7 +2934,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="9">
         <v>3</v>
@@ -2528,7 +2944,7 @@
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="9">
         <v>94</v>
@@ -2538,7 +2954,7 @@
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J16" s="10">
         <v>1</v>
@@ -2548,7 +2964,7 @@
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N16" s="9">
         <v>9</v>
@@ -2559,7 +2975,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" s="10">
         <v>14</v>
@@ -2573,7 +2989,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="8"/>
       <c r="I17" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J17" s="9">
         <v>8</v>
@@ -2583,7 +2999,7 @@
       </c>
       <c r="L17" s="8"/>
       <c r="M17" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N17" s="9">
         <v>2</v>
@@ -2594,7 +3010,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="9">
         <v>2</v>
@@ -2608,7 +3024,7 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J18" s="9">
         <v>2</v>
@@ -2618,7 +3034,7 @@
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N18" s="9">
         <v>16</v>
@@ -2629,7 +3045,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" s="9">
         <v>0</v>
@@ -2643,7 +3059,7 @@
       <c r="G19" s="10"/>
       <c r="H19" s="8"/>
       <c r="I19" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J19" s="9">
         <v>4</v>
@@ -2653,7 +3069,7 @@
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N19" s="9">
         <v>96</v>
@@ -2664,7 +3080,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="9">
         <v>23</v>
@@ -2678,7 +3094,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J20" s="9">
         <v>6</v>
@@ -2693,7 +3109,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21" s="10">
         <v>3</v>
@@ -2707,7 +3123,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J21" s="9">
         <v>6</v>
@@ -2722,7 +3138,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B22" s="9">
         <v>9</v>
@@ -2736,7 +3152,7 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J22" s="10">
         <v>15</v>
@@ -2751,7 +3167,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B23" s="9">
         <v>1</v>
@@ -2765,7 +3181,7 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J23" s="10">
         <v>2</v>
@@ -2780,7 +3196,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
@@ -2794,7 +3210,7 @@
       <c r="G24" s="10"/>
       <c r="H24" s="8"/>
       <c r="I24" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J24" s="10">
         <v>7</v>
@@ -2809,7 +3225,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="10">
         <v>120</v>
@@ -2823,7 +3239,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J25" s="10">
         <v>19</v>
@@ -2846,7 +3262,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J26" s="9">
         <v>3</v>
@@ -2869,7 +3285,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J27" s="9">
         <v>3</v>
@@ -2892,7 +3308,7 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J28" s="10">
         <v>1</v>
@@ -2915,7 +3331,7 @@
       <c r="G29" s="10"/>
       <c r="H29" s="8"/>
       <c r="I29" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J29" s="10">
         <v>15</v>
@@ -2938,7 +3354,7 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J30" s="9">
         <v>2</v>
@@ -2961,7 +3377,7 @@
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J31" s="9">
         <v>7</v>
@@ -2981,7 +3397,7 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J32" s="10">
         <v>168</v>
@@ -3044,13 +3460,13 @@
         <v>19</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
@@ -3059,7 +3475,7 @@
       </c>
       <c r="B2" s="6">
         <f>COUNTIF(掠夺总榜!A$1:S$150,$A2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="4">
         <f>COUNTIF(盟会战!A$1:Q$150,$A2)</f>
@@ -3071,15 +3487,15 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:D2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="4">
         <f>IF($E2&gt;6,6,$E2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="4">
         <f>SUM(G2:G140)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2" s="4">
         <f>SUM(E2:E140)-I2</f>
@@ -3129,13 +3545,13 @@
         <v>19</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
@@ -3197,14 +3613,14 @@
         <v>19</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -3277,13 +3693,13 @@
         <v>19</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
@@ -3326,13 +3742,13 @@
         <v>6</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>('逐梦-箱子'!$I$2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3">
         <f>('如梦-箱子'!$I$2)</f>
@@ -3348,7 +3764,7 @@
       </c>
       <c r="E2" s="3">
         <f>SUM(A2:D2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>